<commit_message>
ajout calcul coef des IAs
Ajout du calcul de la matrice des coeficient des differentes IA,
correction du bug qui faisait que tous les coef list n'étaient pas sur tous les edges
</commit_message>
<xml_diff>
--- a/Weight_matrix.xlsx
+++ b/Weight_matrix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\ai-sustainability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B61DBE-1522-44F9-966F-11CD53CE0B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAE9F8-0B13-45A3-A5B2-4AE0FC8C3D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
   </bookViews>
@@ -691,7 +691,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -709,10 +709,10 @@
         <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -930,11 +930,11 @@
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
Return the n best AIs
</commit_message>
<xml_diff>
--- a/Weight_matrix.xlsx
+++ b/Weight_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hennecarta\Documents\Graph_decision_AI\ai-sustainability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BAE9F8-0B13-45A3-A5B2-4AE0FC8C3D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB69BE0D-46C9-4D72-B7B7-1A50278BF59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC26B5E7-4148-4700-AAF1-8A62823EFFAF}"/>
   </bookViews>
@@ -691,7 +691,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>